<commit_message>
Updated README.md - Updated Vocabularies - Added command for FreeBase - Removed old files
</commit_message>
<xml_diff>
--- a/otherVocabs.xlsx
+++ b/otherVocabs.xlsx
@@ -5,16 +5,15 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marco\Desktop\Internship\Results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marco\Desktop\Internship\KnowDive\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A2D745D-E9C7-4531-927B-89770B381011}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2CA2872-9847-4DB0-ABAD-1D6AC61134DB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
-    <sheet name="Results" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -29,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="158">
   <si>
     <t>Link</t>
   </si>
@@ -205,12 +204,6 @@
     <t>Folder</t>
   </si>
   <si>
-    <t>C:\Users\marco\Desktop\Internship\Results</t>
-  </si>
-  <si>
-    <t>other_Vocabs</t>
-  </si>
-  <si>
     <t>gist by Semantic Arts, Inc.</t>
   </si>
   <si>
@@ -274,9 +267,6 @@
     <t>gistDeprecated</t>
   </si>
   <si>
-    <t>English</t>
-  </si>
-  <si>
     <t>http://ontologies.semanticarts.com/o/gistDeprecated8.0.0.owl</t>
   </si>
   <si>
@@ -421,21 +411,6 @@
     <t>v3.9</t>
   </si>
   <si>
-    <t>WordNet-OWL</t>
-  </si>
-  <si>
-    <t>http://www.adampease.org/OP/WordNet.owl</t>
-  </si>
-  <si>
-    <t>http://www.ontologyportal.org/WordNet.owl#</t>
-  </si>
-  <si>
-    <t>v3.0</t>
-  </si>
-  <si>
-    <t>2010-05-10</t>
-  </si>
-  <si>
     <t>v1.6</t>
   </si>
   <si>
@@ -460,9 +435,6 @@
     <t>kbpedia_reference_concepts_linkage_inferrence_extended</t>
   </si>
   <si>
-    <t>file:///{Path_to_uncompressed_file}</t>
-  </si>
-  <si>
     <t>2019-01-19</t>
   </si>
   <si>
@@ -515,6 +487,21 @@
   </si>
   <si>
     <t>https://raw.githubusercontent.com/knowdive/resources/master/Vocabularies/DOLCE/TemporalRelations.owl</t>
+  </si>
+  <si>
+    <t>en</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/knowdive/resources/master/Vocabularies/KBPedia/kbpedia_reference_concepts_linkage.n3</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/knowdive/resources/master/Vocabularies/FreeBase/FreeBaseSchema.nt</t>
+  </si>
+  <si>
+    <t>FreeBaseSchema</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/BFO-ontology/BFO/master/ro.owl</t>
   </si>
 </sst>
 </file>
@@ -936,8 +923,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I657"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D16" workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -984,1152 +971,1121 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>90</v>
+        <v>8</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>60</v>
       </c>
       <c r="C2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2" t="s">
+        <v>153</v>
+      </c>
+      <c r="E2" t="s">
         <v>83</v>
       </c>
-      <c r="D2" t="s">
-        <v>81</v>
-      </c>
-      <c r="E2" t="s">
-        <v>94</v>
-      </c>
       <c r="F2" s="4" t="s">
-        <v>139</v>
+        <v>84</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>6</v>
+        <v>62</v>
       </c>
       <c r="H2" t="s">
-        <v>5</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>89</v>
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>60</v>
       </c>
       <c r="C3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D3" t="s">
+        <v>153</v>
+      </c>
+      <c r="E3" t="s">
+        <v>83</v>
+      </c>
+      <c r="F3" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="D3" t="s">
-        <v>81</v>
-      </c>
-      <c r="E3" t="s">
-        <v>85</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>88</v>
-      </c>
       <c r="G3" s="1" t="s">
-        <v>150</v>
+        <v>63</v>
       </c>
       <c r="H3" t="s">
-        <v>113</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D4" t="s">
-        <v>81</v>
+        <v>153</v>
       </c>
       <c r="E4" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>64</v>
       </c>
       <c r="H4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D5" t="s">
-        <v>81</v>
+        <v>153</v>
       </c>
       <c r="E5" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>65</v>
       </c>
       <c r="H5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D6" t="s">
-        <v>81</v>
+        <v>153</v>
       </c>
       <c r="E6" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="H6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D7" t="s">
-        <v>81</v>
+        <v>153</v>
       </c>
       <c r="E7" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C8" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D8" t="s">
-        <v>81</v>
+        <v>153</v>
       </c>
       <c r="E8" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="H8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C9" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D9" t="s">
-        <v>81</v>
+        <v>153</v>
       </c>
       <c r="E9" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>68</v>
       </c>
       <c r="H9" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C10" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D10" t="s">
-        <v>81</v>
+        <v>153</v>
       </c>
       <c r="E10" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>69</v>
       </c>
       <c r="H10" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C11" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D11" t="s">
-        <v>81</v>
+        <v>153</v>
       </c>
       <c r="E11" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>70</v>
       </c>
       <c r="H11" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C12" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D12" t="s">
-        <v>81</v>
+        <v>153</v>
       </c>
       <c r="E12" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>71</v>
       </c>
       <c r="H12" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C13" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D13" t="s">
-        <v>81</v>
+        <v>153</v>
       </c>
       <c r="E13" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>72</v>
       </c>
       <c r="H13" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C14" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D14" t="s">
-        <v>81</v>
+        <v>153</v>
       </c>
       <c r="E14" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>73</v>
       </c>
       <c r="H14" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C15" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D15" t="s">
-        <v>81</v>
+        <v>153</v>
       </c>
       <c r="E15" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>74</v>
       </c>
       <c r="H15" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C16" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D16" t="s">
-        <v>81</v>
+        <v>153</v>
       </c>
       <c r="E16" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="H16" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C17" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D17" t="s">
-        <v>81</v>
+        <v>153</v>
       </c>
       <c r="E17" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H17" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C18" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D18" t="s">
-        <v>81</v>
+        <v>153</v>
       </c>
       <c r="E18" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="H18" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" t="s">
-        <v>23</v>
+        <v>78</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C19" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D19" t="s">
-        <v>81</v>
+        <v>153</v>
       </c>
       <c r="E19" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="H19" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" t="s">
-        <v>24</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>62</v>
+        <v>1</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>106</v>
       </c>
       <c r="C20" t="s">
-        <v>60</v>
+        <v>104</v>
       </c>
       <c r="D20" t="s">
-        <v>81</v>
+        <v>153</v>
       </c>
       <c r="E20" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>87</v>
+        <v>108</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>78</v>
+        <v>4</v>
       </c>
       <c r="H20" t="s">
-        <v>61</v>
+        <v>96</v>
       </c>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" t="s">
-        <v>80</v>
+        <v>3</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>62</v>
+        <v>105</v>
       </c>
       <c r="C21" t="s">
-        <v>60</v>
+        <v>107</v>
       </c>
       <c r="D21" t="s">
-        <v>81</v>
+        <v>153</v>
       </c>
       <c r="E21" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>87</v>
+        <v>109</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>82</v>
+        <v>2</v>
       </c>
       <c r="H21" t="s">
-        <v>61</v>
+        <v>96</v>
       </c>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" t="s">
-        <v>1</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="C22" t="s">
-        <v>107</v>
+        <v>41</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>113</v>
       </c>
       <c r="D22" t="s">
-        <v>81</v>
+        <v>153</v>
       </c>
       <c r="E22" t="s">
-        <v>94</v>
+        <v>126</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>111</v>
+        <v>125</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="H22" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" t="s">
-        <v>3</v>
+        <v>40</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="C23" t="s">
-        <v>110</v>
+        <v>117</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>113</v>
       </c>
       <c r="D23" t="s">
-        <v>81</v>
+        <v>153</v>
       </c>
       <c r="E23" t="s">
-        <v>94</v>
+        <v>126</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>112</v>
+        <v>125</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>2</v>
+        <v>147</v>
       </c>
       <c r="H23" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>25</v>
+        <v>120</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D24" t="s">
-        <v>81</v>
+        <v>153</v>
       </c>
       <c r="E24" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>25</v>
+        <v>142</v>
       </c>
       <c r="H24" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="25" spans="1:8">
       <c r="A25" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D25" t="s">
-        <v>81</v>
+        <v>153</v>
       </c>
       <c r="E25" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
       <c r="H25" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D26" t="s">
-        <v>81</v>
+        <v>153</v>
       </c>
       <c r="E26" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="H26" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="27" spans="1:8">
       <c r="A27" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D27" t="s">
-        <v>81</v>
+        <v>153</v>
       </c>
       <c r="E27" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="H27" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="28" spans="1:8">
       <c r="A28" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B28" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="D28" t="s">
+        <v>153</v>
+      </c>
+      <c r="E28" t="s">
+        <v>126</v>
+      </c>
+      <c r="F28" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="C28" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="D28" t="s">
-        <v>81</v>
-      </c>
-      <c r="E28" t="s">
-        <v>129</v>
-      </c>
-      <c r="F28" s="4" t="s">
-        <v>128</v>
-      </c>
       <c r="G28" s="1" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="H28" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="29" spans="1:8">
       <c r="A29" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D29" t="s">
-        <v>81</v>
+        <v>153</v>
       </c>
       <c r="E29" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>159</v>
+        <v>145</v>
       </c>
       <c r="H29" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D30" t="s">
-        <v>81</v>
+        <v>153</v>
       </c>
       <c r="E30" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="H30" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="31" spans="1:8">
       <c r="A31" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D31" t="s">
-        <v>81</v>
+        <v>153</v>
       </c>
       <c r="E31" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H31" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="32" spans="1:8">
       <c r="A32" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B32" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="D32" t="s">
+        <v>153</v>
+      </c>
+      <c r="E32" t="s">
         <v>126</v>
       </c>
-      <c r="C32" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="D32" t="s">
-        <v>81</v>
-      </c>
-      <c r="E32" t="s">
-        <v>129</v>
-      </c>
       <c r="F32" s="4" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
       <c r="H32" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="33" spans="1:8">
       <c r="A33" t="s">
-        <v>49</v>
+        <v>26</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D33" t="s">
-        <v>81</v>
+        <v>153</v>
       </c>
       <c r="E33" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>161</v>
+        <v>144</v>
       </c>
       <c r="H33" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="34" spans="1:8">
       <c r="A34" t="s">
-        <v>50</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="C34" s="7" t="s">
-        <v>116</v>
+        <v>29</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="C34" t="s">
+        <v>103</v>
       </c>
       <c r="D34" t="s">
-        <v>81</v>
+        <v>153</v>
       </c>
       <c r="E34" t="s">
-        <v>129</v>
+        <v>102</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>128</v>
+        <v>101</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>158</v>
+        <v>30</v>
       </c>
       <c r="H34" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="35" spans="1:8">
       <c r="A35" t="s">
-        <v>26</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="C35" s="7" t="s">
-        <v>116</v>
+        <v>31</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="C35" t="s">
+        <v>100</v>
       </c>
       <c r="D35" t="s">
-        <v>81</v>
+        <v>153</v>
       </c>
       <c r="E35" t="s">
-        <v>129</v>
+        <v>98</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>128</v>
+        <v>89</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>153</v>
+        <v>32</v>
       </c>
       <c r="H35" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="36" spans="1:8">
       <c r="A36" t="s">
-        <v>27</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>28</v>
+        <v>33</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>90</v>
       </c>
       <c r="C36" t="s">
-        <v>115</v>
+        <v>93</v>
       </c>
       <c r="D36" t="s">
-        <v>81</v>
+        <v>153</v>
       </c>
       <c r="E36" t="s">
-        <v>114</v>
+        <v>91</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="G36" s="1" t="s">
-        <v>28</v>
+        <v>92</v>
+      </c>
+      <c r="G36" s="6" t="s">
+        <v>157</v>
       </c>
       <c r="H36" t="s">
-        <v>27</v>
+        <v>95</v>
       </c>
     </row>
     <row r="37" spans="1:8">
       <c r="A37" t="s">
-        <v>29</v>
-      </c>
-      <c r="B37" s="5" t="s">
-        <v>102</v>
+        <v>37</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>128</v>
       </c>
       <c r="C37" t="s">
-        <v>106</v>
+        <v>129</v>
       </c>
       <c r="D37" t="s">
-        <v>81</v>
+        <v>153</v>
       </c>
       <c r="E37" t="s">
-        <v>105</v>
+        <v>127</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>104</v>
+        <v>130</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="H37" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="38" spans="1:8">
       <c r="A38" t="s">
-        <v>31</v>
-      </c>
-      <c r="B38" s="5" t="s">
-        <v>102</v>
+        <v>35</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>36</v>
       </c>
       <c r="C38" t="s">
-        <v>103</v>
+        <v>129</v>
       </c>
       <c r="D38" t="s">
-        <v>81</v>
+        <v>153</v>
       </c>
       <c r="E38" t="s">
-        <v>101</v>
+        <v>127</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>92</v>
+        <v>130</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="H38" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="39" spans="1:8">
       <c r="A39" t="s">
-        <v>33</v>
-      </c>
-      <c r="B39" s="5" t="s">
-        <v>93</v>
+        <v>38</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>39</v>
       </c>
       <c r="C39" t="s">
-        <v>96</v>
+        <v>129</v>
       </c>
       <c r="D39" t="s">
-        <v>81</v>
+        <v>153</v>
       </c>
       <c r="E39" t="s">
+        <v>127</v>
+      </c>
+      <c r="F39" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H39" t="s">
         <v>94</v>
-      </c>
-      <c r="F39" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="G39" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="H39" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="40" spans="1:8">
       <c r="A40" t="s">
-        <v>37</v>
+        <v>134</v>
       </c>
       <c r="B40" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C40" t="s">
+        <v>134</v>
+      </c>
+      <c r="D40" t="s">
+        <v>153</v>
+      </c>
+      <c r="E40" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="C40" t="s">
-        <v>137</v>
-      </c>
-      <c r="D40" t="s">
-        <v>81</v>
-      </c>
-      <c r="E40" t="s">
+      <c r="F40" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="F40" s="4" t="s">
-        <v>138</v>
-      </c>
       <c r="G40" s="1" t="s">
-        <v>34</v>
+        <v>154</v>
       </c>
       <c r="H40" t="s">
-        <v>97</v>
+        <v>132</v>
       </c>
     </row>
     <row r="41" spans="1:8">
       <c r="A41" t="s">
-        <v>35</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>36</v>
+        <v>137</v>
+      </c>
+      <c r="B41" t="s">
+        <v>140</v>
       </c>
       <c r="C41" t="s">
+        <v>156</v>
+      </c>
+      <c r="D41" t="s">
+        <v>153</v>
+      </c>
+      <c r="E41" t="s">
+        <v>138</v>
+      </c>
+      <c r="F41" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="H41" t="s">
         <v>137</v>
-      </c>
-      <c r="D41" t="s">
-        <v>81</v>
-      </c>
-      <c r="E41" t="s">
-        <v>135</v>
-      </c>
-      <c r="F41" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="G41" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="H41" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="42" spans="1:8">
       <c r="A42" t="s">
-        <v>38</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>39</v>
+        <v>5</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>87</v>
       </c>
       <c r="C42" t="s">
-        <v>137</v>
+        <v>80</v>
       </c>
       <c r="D42" t="s">
-        <v>81</v>
+        <v>153</v>
       </c>
       <c r="E42" t="s">
-        <v>135</v>
+        <v>91</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>39</v>
+        <v>6</v>
       </c>
       <c r="H42" t="s">
-        <v>97</v>
+        <v>5</v>
       </c>
     </row>
     <row r="43" spans="1:8">
       <c r="A43" t="s">
-        <v>130</v>
-      </c>
-      <c r="B43" s="5" t="s">
-        <v>132</v>
+        <v>7</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>86</v>
       </c>
       <c r="C43" t="s">
-        <v>97</v>
+        <v>81</v>
       </c>
       <c r="D43" t="s">
-        <v>81</v>
+        <v>153</v>
       </c>
       <c r="E43" t="s">
-        <v>133</v>
+        <v>82</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="G43" t="s">
-        <v>131</v>
+        <v>85</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>141</v>
       </c>
       <c r="H43" t="s">
-        <v>97</v>
+        <v>110</v>
       </c>
     </row>
     <row r="44" spans="1:8">
       <c r="A44" t="s">
-        <v>142</v>
+        <v>27</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>141</v>
+        <v>28</v>
       </c>
       <c r="C44" t="s">
-        <v>142</v>
+        <v>112</v>
       </c>
       <c r="D44" t="s">
-        <v>81</v>
-      </c>
-      <c r="E44" s="4" t="s">
-        <v>145</v>
+        <v>153</v>
+      </c>
+      <c r="E44" t="s">
+        <v>111</v>
       </c>
       <c r="F44" s="4" t="s">
-        <v>144</v>
+        <v>88</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>143</v>
+        <v>28</v>
       </c>
       <c r="H44" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8">
-      <c r="A45" t="s">
-        <v>146</v>
-      </c>
-      <c r="B45" t="s">
-        <v>149</v>
-      </c>
-      <c r="C45" t="s">
-        <v>146</v>
-      </c>
-      <c r="D45" t="s">
-        <v>81</v>
-      </c>
-      <c r="E45" t="s">
-        <v>147</v>
-      </c>
-      <c r="F45" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="G45" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="H45" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8">
-      <c r="B47" s="1"/>
-      <c r="F47" s="4"/>
-      <c r="G47" s="1"/>
+        <v>27</v>
+      </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" s="3"/>
@@ -4569,46 +4525,22 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B4" r:id="rId1" display="http://www.semanticarts.com/gist/" xr:uid="{FA71FE71-B564-4416-ACA8-8A4A9C372B82}"/>
-    <hyperlink ref="B5:B20" r:id="rId2" display="http://www.semanticarts.com/gist/" xr:uid="{3A3EAF8B-638F-4A5E-B346-35063737FFAE}"/>
-    <hyperlink ref="B21" r:id="rId3" display="http://www.semanticarts.com/gist/" xr:uid="{EE1FF1D1-BD1F-43CF-ADB1-AAC32E98343E}"/>
-    <hyperlink ref="B3" r:id="rId4" xr:uid="{D4A7064B-307D-496F-9971-B2B3A0105BA0}"/>
-    <hyperlink ref="G39" r:id="rId5" xr:uid="{1BB698E5-DE47-48B1-A577-06F8BA6700C2}"/>
-    <hyperlink ref="B23" r:id="rId6" xr:uid="{04B38C27-8E79-4151-BA7D-6085080F35B7}"/>
-    <hyperlink ref="B41" r:id="rId7" xr:uid="{1AFED0F6-A06D-46C9-817D-191603D9E370}"/>
-    <hyperlink ref="B36" r:id="rId8" xr:uid="{981530C9-CA3A-49CA-8C93-60FC320619AB}"/>
-    <hyperlink ref="B29" r:id="rId9" xr:uid="{A7AB9614-93CE-476E-A33D-D82328BD1669}"/>
-    <hyperlink ref="B27" r:id="rId10" xr:uid="{E334D193-1C74-47FD-A8F6-2E7AAD543463}"/>
-    <hyperlink ref="G40" r:id="rId11" xr:uid="{0C2097A0-DB18-4CC6-B00F-19795B355C5F}"/>
+    <hyperlink ref="B2" r:id="rId1" display="http://www.semanticarts.com/gist/" xr:uid="{FA71FE71-B564-4416-ACA8-8A4A9C372B82}"/>
+    <hyperlink ref="B3:B18" r:id="rId2" display="http://www.semanticarts.com/gist/" xr:uid="{3A3EAF8B-638F-4A5E-B346-35063737FFAE}"/>
+    <hyperlink ref="B19" r:id="rId3" display="http://www.semanticarts.com/gist/" xr:uid="{EE1FF1D1-BD1F-43CF-ADB1-AAC32E98343E}"/>
+    <hyperlink ref="B43" r:id="rId4" xr:uid="{D4A7064B-307D-496F-9971-B2B3A0105BA0}"/>
+    <hyperlink ref="G36" r:id="rId5" xr:uid="{1BB698E5-DE47-48B1-A577-06F8BA6700C2}"/>
+    <hyperlink ref="B21" r:id="rId6" xr:uid="{04B38C27-8E79-4151-BA7D-6085080F35B7}"/>
+    <hyperlink ref="B38" r:id="rId7" xr:uid="{1AFED0F6-A06D-46C9-817D-191603D9E370}"/>
+    <hyperlink ref="B44" r:id="rId8" xr:uid="{981530C9-CA3A-49CA-8C93-60FC320619AB}"/>
+    <hyperlink ref="B27" r:id="rId9" xr:uid="{A7AB9614-93CE-476E-A33D-D82328BD1669}"/>
+    <hyperlink ref="B25" r:id="rId10" xr:uid="{E334D193-1C74-47FD-A8F6-2E7AAD543463}"/>
+    <hyperlink ref="G37" r:id="rId11" xr:uid="{0C2097A0-DB18-4CC6-B00F-19795B355C5F}"/>
+    <hyperlink ref="G33" r:id="rId12" xr:uid="{3B5219B3-695A-4F3E-9076-0571846FE17D}"/>
+    <hyperlink ref="G40" r:id="rId13" xr:uid="{63EA36A8-7BC3-457C-BD62-3F70E26953DB}"/>
+    <hyperlink ref="G41" r:id="rId14" xr:uid="{7632A022-94E3-4D8B-A48E-9C56A36C5C51}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId12"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCB7F15E-71FF-4B65-97E7-6B348A040F7D}">
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="46" customWidth="1"/>
-    <col min="2" max="2" width="41.28515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId15"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated otherVocabs - Updated KnowledgeFull - Updated KnowledgeLatest
</commit_message>
<xml_diff>
--- a/otherVocabs.xlsx
+++ b/otherVocabs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marco\Desktop\Internship\KnowDive\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2CA2872-9847-4DB0-ABAD-1D6AC61134DB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45A3DBB2-095B-42CC-BE2F-9C0603086241}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -432,9 +432,6 @@
     <t>http://kbpedia.org/kko/rc/</t>
   </si>
   <si>
-    <t>kbpedia_reference_concepts_linkage_inferrence_extended</t>
-  </si>
-  <si>
     <t>2019-01-19</t>
   </si>
   <si>
@@ -502,6 +499,9 @@
   </si>
   <si>
     <t>https://raw.githubusercontent.com/BFO-ontology/BFO/master/ro.owl</t>
+  </si>
+  <si>
+    <t>kbpedia_reference_concepts_linkage</t>
   </si>
 </sst>
 </file>
@@ -923,8 +923,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I657"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -935,7 +935,7 @@
     <col min="4" max="4" width="55.7109375" customWidth="1"/>
     <col min="5" max="5" width="36.7109375" customWidth="1"/>
     <col min="6" max="6" width="27.140625" customWidth="1"/>
-    <col min="7" max="7" width="86.140625" customWidth="1"/>
+    <col min="7" max="7" width="102.28515625" customWidth="1"/>
     <col min="8" max="8" width="18.85546875" customWidth="1"/>
     <col min="9" max="9" width="30.85546875" customWidth="1"/>
   </cols>
@@ -980,7 +980,7 @@
         <v>58</v>
       </c>
       <c r="D2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E2" t="s">
         <v>83</v>
@@ -1006,7 +1006,7 @@
         <v>58</v>
       </c>
       <c r="D3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E3" t="s">
         <v>83</v>
@@ -1032,7 +1032,7 @@
         <v>58</v>
       </c>
       <c r="D4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E4" t="s">
         <v>83</v>
@@ -1058,7 +1058,7 @@
         <v>58</v>
       </c>
       <c r="D5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E5" t="s">
         <v>83</v>
@@ -1084,7 +1084,7 @@
         <v>58</v>
       </c>
       <c r="D6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E6" t="s">
         <v>83</v>
@@ -1110,7 +1110,7 @@
         <v>58</v>
       </c>
       <c r="D7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E7" t="s">
         <v>83</v>
@@ -1136,7 +1136,7 @@
         <v>58</v>
       </c>
       <c r="D8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E8" t="s">
         <v>83</v>
@@ -1162,7 +1162,7 @@
         <v>58</v>
       </c>
       <c r="D9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E9" t="s">
         <v>83</v>
@@ -1188,7 +1188,7 @@
         <v>58</v>
       </c>
       <c r="D10" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E10" t="s">
         <v>83</v>
@@ -1214,7 +1214,7 @@
         <v>58</v>
       </c>
       <c r="D11" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E11" t="s">
         <v>83</v>
@@ -1240,7 +1240,7 @@
         <v>58</v>
       </c>
       <c r="D12" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E12" t="s">
         <v>83</v>
@@ -1266,7 +1266,7 @@
         <v>58</v>
       </c>
       <c r="D13" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E13" t="s">
         <v>83</v>
@@ -1292,7 +1292,7 @@
         <v>58</v>
       </c>
       <c r="D14" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E14" t="s">
         <v>83</v>
@@ -1318,7 +1318,7 @@
         <v>58</v>
       </c>
       <c r="D15" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E15" t="s">
         <v>83</v>
@@ -1344,7 +1344,7 @@
         <v>58</v>
       </c>
       <c r="D16" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E16" t="s">
         <v>83</v>
@@ -1370,7 +1370,7 @@
         <v>58</v>
       </c>
       <c r="D17" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E17" t="s">
         <v>83</v>
@@ -1396,7 +1396,7 @@
         <v>58</v>
       </c>
       <c r="D18" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E18" t="s">
         <v>83</v>
@@ -1422,7 +1422,7 @@
         <v>58</v>
       </c>
       <c r="D19" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E19" t="s">
         <v>83</v>
@@ -1448,7 +1448,7 @@
         <v>104</v>
       </c>
       <c r="D20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E20" t="s">
         <v>91</v>
@@ -1474,7 +1474,7 @@
         <v>107</v>
       </c>
       <c r="D21" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E21" t="s">
         <v>91</v>
@@ -1500,7 +1500,7 @@
         <v>113</v>
       </c>
       <c r="D22" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E22" t="s">
         <v>126</v>
@@ -1526,7 +1526,7 @@
         <v>113</v>
       </c>
       <c r="D23" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E23" t="s">
         <v>126</v>
@@ -1535,7 +1535,7 @@
         <v>125</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H23" t="s">
         <v>97</v>
@@ -1552,7 +1552,7 @@
         <v>113</v>
       </c>
       <c r="D24" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E24" t="s">
         <v>126</v>
@@ -1561,7 +1561,7 @@
         <v>125</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H24" t="s">
         <v>97</v>
@@ -1578,7 +1578,7 @@
         <v>113</v>
       </c>
       <c r="D25" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E25" t="s">
         <v>126</v>
@@ -1587,7 +1587,7 @@
         <v>125</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H25" t="s">
         <v>97</v>
@@ -1604,7 +1604,7 @@
         <v>113</v>
       </c>
       <c r="D26" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E26" t="s">
         <v>126</v>
@@ -1613,7 +1613,7 @@
         <v>125</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H26" t="s">
         <v>97</v>
@@ -1630,7 +1630,7 @@
         <v>113</v>
       </c>
       <c r="D27" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E27" t="s">
         <v>126</v>
@@ -1639,7 +1639,7 @@
         <v>125</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H27" t="s">
         <v>97</v>
@@ -1656,7 +1656,7 @@
         <v>113</v>
       </c>
       <c r="D28" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E28" t="s">
         <v>126</v>
@@ -1665,7 +1665,7 @@
         <v>125</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H28" t="s">
         <v>97</v>
@@ -1682,7 +1682,7 @@
         <v>113</v>
       </c>
       <c r="D29" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E29" t="s">
         <v>126</v>
@@ -1691,7 +1691,7 @@
         <v>125</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H29" t="s">
         <v>97</v>
@@ -1708,7 +1708,7 @@
         <v>113</v>
       </c>
       <c r="D30" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E30" t="s">
         <v>126</v>
@@ -1717,7 +1717,7 @@
         <v>125</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H30" t="s">
         <v>97</v>
@@ -1734,7 +1734,7 @@
         <v>113</v>
       </c>
       <c r="D31" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E31" t="s">
         <v>126</v>
@@ -1743,7 +1743,7 @@
         <v>125</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H31" t="s">
         <v>97</v>
@@ -1760,7 +1760,7 @@
         <v>113</v>
       </c>
       <c r="D32" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E32" t="s">
         <v>126</v>
@@ -1769,7 +1769,7 @@
         <v>125</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H32" t="s">
         <v>97</v>
@@ -1786,7 +1786,7 @@
         <v>113</v>
       </c>
       <c r="D33" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E33" t="s">
         <v>126</v>
@@ -1795,7 +1795,7 @@
         <v>125</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H33" t="s">
         <v>97</v>
@@ -1812,7 +1812,7 @@
         <v>103</v>
       </c>
       <c r="D34" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E34" t="s">
         <v>102</v>
@@ -1838,7 +1838,7 @@
         <v>100</v>
       </c>
       <c r="D35" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E35" t="s">
         <v>98</v>
@@ -1864,7 +1864,7 @@
         <v>93</v>
       </c>
       <c r="D36" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E36" t="s">
         <v>91</v>
@@ -1873,7 +1873,7 @@
         <v>92</v>
       </c>
       <c r="G36" s="6" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H36" t="s">
         <v>95</v>
@@ -1890,7 +1890,7 @@
         <v>129</v>
       </c>
       <c r="D37" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E37" t="s">
         <v>127</v>
@@ -1916,7 +1916,7 @@
         <v>129</v>
       </c>
       <c r="D38" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E38" t="s">
         <v>127</v>
@@ -1942,7 +1942,7 @@
         <v>129</v>
       </c>
       <c r="D39" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E39" t="s">
         <v>127</v>
@@ -1959,25 +1959,25 @@
     </row>
     <row r="40" spans="1:8">
       <c r="A40" t="s">
-        <v>134</v>
+        <v>157</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>133</v>
       </c>
       <c r="C40" t="s">
+        <v>157</v>
+      </c>
+      <c r="D40" t="s">
+        <v>152</v>
+      </c>
+      <c r="E40" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="F40" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="D40" t="s">
+      <c r="G40" s="1" t="s">
         <v>153</v>
-      </c>
-      <c r="E40" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="F40" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="G40" s="1" t="s">
-        <v>154</v>
       </c>
       <c r="H40" t="s">
         <v>132</v>
@@ -1985,28 +1985,28 @@
     </row>
     <row r="41" spans="1:8">
       <c r="A41" t="s">
+        <v>136</v>
+      </c>
+      <c r="B41" t="s">
+        <v>139</v>
+      </c>
+      <c r="C41" t="s">
+        <v>155</v>
+      </c>
+      <c r="D41" t="s">
+        <v>152</v>
+      </c>
+      <c r="E41" t="s">
         <v>137</v>
       </c>
-      <c r="B41" t="s">
-        <v>140</v>
-      </c>
-      <c r="C41" t="s">
-        <v>156</v>
-      </c>
-      <c r="D41" t="s">
-        <v>153</v>
-      </c>
-      <c r="E41" t="s">
+      <c r="F41" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="F41" s="4" t="s">
-        <v>139</v>
-      </c>
       <c r="G41" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H41" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="42" spans="1:8">
@@ -2020,7 +2020,7 @@
         <v>80</v>
       </c>
       <c r="D42" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E42" t="s">
         <v>91</v>
@@ -2046,7 +2046,7 @@
         <v>81</v>
       </c>
       <c r="D43" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E43" t="s">
         <v>82</v>
@@ -2055,7 +2055,7 @@
         <v>85</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H43" t="s">
         <v>110</v>
@@ -2072,7 +2072,7 @@
         <v>112</v>
       </c>
       <c r="D44" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E44" t="s">
         <v>111</v>

</xml_diff>